<commit_message>
Ready to prepare test measurepower
</commit_message>
<xml_diff>
--- a/arduino_to_wiseserver.xlsx
+++ b/arduino_to_wiseserver.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="141">
   <si>
     <t>Leftwaist_P</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>18 0</t>
+  </si>
+  <si>
+    <t>17 260</t>
+  </si>
+  <si>
+    <t>19 1223</t>
+  </si>
+  <si>
+    <t>20 1635</t>
+  </si>
+  <si>
+    <t>21 2861</t>
+  </si>
+  <si>
+    <t>22 3172</t>
+  </si>
+  <si>
+    <t>23 3578</t>
+  </si>
+  <si>
+    <t>24 4089</t>
+  </si>
+  <si>
+    <t>25 4811</t>
+  </si>
+  <si>
+    <t>26 5320</t>
+  </si>
+  <si>
+    <t>27 5726</t>
+  </si>
+  <si>
+    <t>28 6040</t>
+  </si>
+  <si>
+    <t>29 7363</t>
+  </si>
+  <si>
+    <t>30 8187</t>
+  </si>
+  <si>
+    <t>31 8899</t>
+  </si>
+  <si>
+    <t>33 12082</t>
+  </si>
+  <si>
+    <t>37 16579</t>
+  </si>
+  <si>
+    <t>39 18217</t>
+  </si>
+  <si>
+    <t>40 18634</t>
+  </si>
+  <si>
+    <t>43 23032</t>
+  </si>
+  <si>
     <t>44 23954</t>
   </si>
   <si>
@@ -169,227 +229,236 @@
   </si>
   <si>
     <t>82 55494</t>
+  </si>
+  <si>
+    <t>2453:11:Q93:BE:A7!11e</t>
+  </si>
+  <si>
+    <t>2869:12:Q93:BE:A7!12e</t>
+  </si>
+  <si>
+    <t>3305:13:Q93:BE:A7!13e</t>
+  </si>
+  <si>
+    <t>3674:14:Q93:BE:A7!14e</t>
+  </si>
+  <si>
+    <t>4554:15:Q93:BE:A7!15e</t>
+  </si>
+  <si>
+    <t>4931:16:Q93:BE:A7!16e</t>
+  </si>
+  <si>
+    <t>5304:17:Q93:BE:A7!17e</t>
+  </si>
+  <si>
+    <t>5738:18:Q93:BE:A7!18e</t>
+  </si>
+  <si>
+    <t>6959:19:Q93:BE:A7!19e</t>
+  </si>
+  <si>
+    <t>7363:20:Q93:BE:A7!20e</t>
+  </si>
+  <si>
+    <t>8569:21:Q93:BE:A7!21e</t>
+  </si>
+  <si>
+    <t>8993:22:Q93:BE:A7!22e</t>
+  </si>
+  <si>
+    <t>9388:23:Q93:BE:A7!23e</t>
+  </si>
+  <si>
+    <t>9829:24:Q93:BE:A7!24e</t>
+  </si>
+  <si>
+    <t>10614:25:Q93:BE:A7!25e</t>
+  </si>
+  <si>
+    <t>11077:26:Q93:BE:A7!26e</t>
+  </si>
+  <si>
+    <t>11446:27:Q93:BE:A7!27e</t>
+  </si>
+  <si>
+    <t>11784:28:Q93:BE:A7!28e</t>
+  </si>
+  <si>
+    <t>13084:29:Q93:BE:A7!29e</t>
+  </si>
+  <si>
+    <t>13839:30:Q93:BE:A7!30e</t>
+  </si>
+  <si>
+    <t>14652:31:Q93:BE:A7!31e</t>
+  </si>
+  <si>
+    <t>15820:32:Q93:BE:A7!32e</t>
+  </si>
+  <si>
+    <t>17904:33:Q93:BE:A7!33e</t>
+  </si>
+  <si>
+    <t>18302:34:Q93:BE:A7!34e</t>
+  </si>
+  <si>
+    <t>18708:35:Q93:BE:A7!35e</t>
+  </si>
+  <si>
+    <t>21106:36:Q93:BE:A7!36e</t>
+  </si>
+  <si>
+    <t>22325:37:Q93:BE:A7!37e</t>
+  </si>
+  <si>
+    <t>23128:38:Q93:BE:A7!38e</t>
+  </si>
+  <si>
+    <t>23949:39:Q93:BE:A7!39e</t>
+  </si>
+  <si>
+    <t>24382:40:Q93:BE:A7!40e</t>
+  </si>
+  <si>
+    <t>26823:41:Q93:BE:A7!41e</t>
+  </si>
+  <si>
+    <t>27238:42:Q93:BE:A7!42e</t>
+  </si>
+  <si>
+    <t>28822:43:Q93:BE:A7!43e</t>
+  </si>
+  <si>
+    <t>29678:44:Q93:BE:A7!44e</t>
+  </si>
+  <si>
+    <t>30072:45:Q93:BE:A7!45e</t>
+  </si>
+  <si>
+    <t>30441:46:Q93:BE:A7!46e</t>
+  </si>
+  <si>
+    <t>32477:47:Q93:BE:A7!47e</t>
+  </si>
+  <si>
+    <t>33276:48:Q93:BE:A7!48e</t>
+  </si>
+  <si>
+    <t>34501:49:Q93:BE:A7!49e</t>
+  </si>
+  <si>
+    <t>34948:50:Q93:BE:A7!50e</t>
+  </si>
+  <si>
+    <t>35325:51:Q93:BE:A7!51e</t>
+  </si>
+  <si>
+    <t>35686:52:Q93:BE:A7!52e</t>
+  </si>
+  <si>
+    <t>36544:53:Q93:BE:A7!53e</t>
+  </si>
+  <si>
+    <t>38943:54:Q93:BE:A7!54e</t>
+  </si>
+  <si>
+    <t>40560:55:Q93:BE:A7!55e</t>
+  </si>
+  <si>
+    <t>40987:56:Q93:BE:A7!56e</t>
+  </si>
+  <si>
+    <t>41804:57:Q93:BE:A7!57e</t>
+  </si>
+  <si>
+    <t>43823:58:Q93:BE:A7!58e</t>
+  </si>
+  <si>
+    <t>44651:59:Q93:BE:A7!59e</t>
+  </si>
+  <si>
+    <t>45847:60:Q93:BE:A7!60e</t>
+  </si>
+  <si>
+    <t>46251:61:Q93:BE:A7!61e</t>
+  </si>
+  <si>
+    <t>47157:62:Q93:BE:A7!62e</t>
+  </si>
+  <si>
+    <t>47568:63:Q93:BE:A7!63e</t>
+  </si>
+  <si>
+    <t>47803:64:Q93:BE:A7!64e</t>
+  </si>
+  <si>
+    <t>49079:65:Q93:BE:A7!65e</t>
+  </si>
+  <si>
+    <t>49607:66:Q93:BE:A7!66e</t>
+  </si>
+  <si>
+    <t>49885:67:Q93:BE:A7!67e</t>
+  </si>
+  <si>
+    <t>51069:68:Q93:BE:A7!68e</t>
+  </si>
+  <si>
+    <t>51479:69:Q93:BE:A7!69e</t>
+  </si>
+  <si>
+    <t>52285:70:Q93:BE:A7!70e</t>
+  </si>
+  <si>
+    <t>52700:71:Q93:BE:A7!71e</t>
+  </si>
+  <si>
+    <t>53506:72:Q93:BE:A7!72e</t>
+  </si>
+  <si>
+    <t>53871:73:Q93:BE:A7!73e</t>
+  </si>
+  <si>
+    <t>54297:74:Q93:BE:A7!74e</t>
+  </si>
+  <si>
+    <t>55140:75:Q93:BE:A7!75e</t>
+  </si>
+  <si>
+    <t>56755:76:Q93:BE:A7!76e</t>
+  </si>
+  <si>
+    <t>58415:77:Q93:BE:A7!77e</t>
+  </si>
+  <si>
+    <t>58745:78:Q93:BE:A7!78e</t>
+  </si>
+  <si>
+    <t>59193:79:Q93:BE:A7!79e</t>
+  </si>
+  <si>
+    <t>60044:80:Q93:BE:A7!80e</t>
+  </si>
+  <si>
+    <t>60507:81:Q93:BE:A7!81e</t>
+  </si>
+  <si>
+    <t>61219:82:Q93:BE:A7!82e</t>
+  </si>
+  <si>
+    <t>data from wise server</t>
+  </si>
+  <si>
+    <t>data from arduino</t>
+  </si>
+  <si>
+    <t>17~30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17 0</t>
+    <t>5738:18:Q93:BE:A7!18e</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2453:11:Q93:BE:A7!11e</t>
-  </si>
-  <si>
-    <t>2869:12:Q93:BE:A7!12e</t>
-  </si>
-  <si>
-    <t>3305:13:Q93:BE:A7!13e</t>
-  </si>
-  <si>
-    <t>3674:14:Q93:BE:A7!14e</t>
-  </si>
-  <si>
-    <t>4554:15:Q93:BE:A7!15e</t>
-  </si>
-  <si>
-    <t>4931:16:Q93:BE:A7!16e</t>
-  </si>
-  <si>
-    <t>5304:17:Q93:BE:A7!17e</t>
-  </si>
-  <si>
-    <t>5738:18:Q93:BE:A7!18e</t>
-  </si>
-  <si>
-    <t>6959:19:Q93:BE:A7!19e</t>
-  </si>
-  <si>
-    <t>7363:20:Q93:BE:A7!20e</t>
-  </si>
-  <si>
-    <t>8569:21:Q93:BE:A7!21e</t>
-  </si>
-  <si>
-    <t>8993:22:Q93:BE:A7!22e</t>
-  </si>
-  <si>
-    <t>9388:23:Q93:BE:A7!23e</t>
-  </si>
-  <si>
-    <t>9829:24:Q93:BE:A7!24e</t>
-  </si>
-  <si>
-    <t>10614:25:Q93:BE:A7!25e</t>
-  </si>
-  <si>
-    <t>11077:26:Q93:BE:A7!26e</t>
-  </si>
-  <si>
-    <t>11446:27:Q93:BE:A7!27e</t>
-  </si>
-  <si>
-    <t>11784:28:Q93:BE:A7!28e</t>
-  </si>
-  <si>
-    <t>13084:29:Q93:BE:A7!29e</t>
-  </si>
-  <si>
-    <t>13839:30:Q93:BE:A7!30e</t>
-  </si>
-  <si>
-    <t>14652:31:Q93:BE:A7!31e</t>
-  </si>
-  <si>
-    <t>15820:32:Q93:BE:A7!32e</t>
-  </si>
-  <si>
-    <t>17904:33:Q93:BE:A7!33e</t>
-  </si>
-  <si>
-    <t>18302:34:Q93:BE:A7!34e</t>
-  </si>
-  <si>
-    <t>18708:35:Q93:BE:A7!35e</t>
-  </si>
-  <si>
-    <t>21106:36:Q93:BE:A7!36e</t>
-  </si>
-  <si>
-    <t>22325:37:Q93:BE:A7!37e</t>
-  </si>
-  <si>
-    <t>23128:38:Q93:BE:A7!38e</t>
-  </si>
-  <si>
-    <t>23949:39:Q93:BE:A7!39e</t>
-  </si>
-  <si>
-    <t>24382:40:Q93:BE:A7!40e</t>
-  </si>
-  <si>
-    <t>26823:41:Q93:BE:A7!41e</t>
-  </si>
-  <si>
-    <t>27238:42:Q93:BE:A7!42e</t>
-  </si>
-  <si>
-    <t>28822:43:Q93:BE:A7!43e</t>
-  </si>
-  <si>
-    <t>29678:44:Q93:BE:A7!44e</t>
-  </si>
-  <si>
-    <t>30072:45:Q93:BE:A7!45e</t>
-  </si>
-  <si>
-    <t>30441:46:Q93:BE:A7!46e</t>
-  </si>
-  <si>
-    <t>32477:47:Q93:BE:A7!47e</t>
-  </si>
-  <si>
-    <t>33276:48:Q93:BE:A7!48e</t>
-  </si>
-  <si>
-    <t>34501:49:Q93:BE:A7!49e</t>
-  </si>
-  <si>
-    <t>34948:50:Q93:BE:A7!50e</t>
-  </si>
-  <si>
-    <t>35325:51:Q93:BE:A7!51e</t>
-  </si>
-  <si>
-    <t>35686:52:Q93:BE:A7!52e</t>
-  </si>
-  <si>
-    <t>36544:53:Q93:BE:A7!53e</t>
-  </si>
-  <si>
-    <t>38943:54:Q93:BE:A7!54e</t>
-  </si>
-  <si>
-    <t>40560:55:Q93:BE:A7!55e</t>
-  </si>
-  <si>
-    <t>40987:56:Q93:BE:A7!56e</t>
-  </si>
-  <si>
-    <t>41804:57:Q93:BE:A7!57e</t>
-  </si>
-  <si>
-    <t>43823:58:Q93:BE:A7!58e</t>
-  </si>
-  <si>
-    <t>44651:59:Q93:BE:A7!59e</t>
-  </si>
-  <si>
-    <t>45847:60:Q93:BE:A7!60e</t>
-  </si>
-  <si>
-    <t>46251:61:Q93:BE:A7!61e</t>
-  </si>
-  <si>
-    <t>47157:62:Q93:BE:A7!62e</t>
-  </si>
-  <si>
-    <t>47568:63:Q93:BE:A7!63e</t>
-  </si>
-  <si>
-    <t>47803:64:Q93:BE:A7!64e</t>
-  </si>
-  <si>
-    <t>49079:65:Q93:BE:A7!65e</t>
-  </si>
-  <si>
-    <t>49607:66:Q93:BE:A7!66e</t>
-  </si>
-  <si>
-    <t>49885:67:Q93:BE:A7!67e</t>
-  </si>
-  <si>
-    <t>51069:68:Q93:BE:A7!68e</t>
-  </si>
-  <si>
-    <t>51479:69:Q93:BE:A7!69e</t>
-  </si>
-  <si>
-    <t>52285:70:Q93:BE:A7!70e</t>
-  </si>
-  <si>
-    <t>52700:71:Q93:BE:A7!71e</t>
-  </si>
-  <si>
-    <t>53506:72:Q93:BE:A7!72e</t>
-  </si>
-  <si>
-    <t>53871:73:Q93:BE:A7!73e</t>
-  </si>
-  <si>
-    <t>54297:74:Q93:BE:A7!74e</t>
-  </si>
-  <si>
-    <t>55140:75:Q93:BE:A7!75e</t>
-  </si>
-  <si>
-    <t>56755:76:Q93:BE:A7!76e</t>
-  </si>
-  <si>
-    <t>58415:77:Q93:BE:A7!77e</t>
-  </si>
-  <si>
-    <t>58745:78:Q93:BE:A7!78e</t>
-  </si>
-  <si>
-    <t>59193:79:Q93:BE:A7!79e</t>
-  </si>
-  <si>
-    <t>60044:80:Q93:BE:A7!80e</t>
-  </si>
-  <si>
-    <t>60507:81:Q93:BE:A7!81e</t>
-  </si>
-  <si>
-    <t>61219:82:Q93:BE:A7!82e</t>
   </si>
 </sst>
 </file>
@@ -474,8 +543,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -518,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="53">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -538,6 +623,14 @@
     <cellStyle name="已瀏覽過的超連結" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -556,6 +649,14 @@
     <cellStyle name="超連結" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="51" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1216,6 +1317,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1259,6 +1361,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1272,6 +1375,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1940,6 +2044,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1977,6 +2082,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1990,6 +2096,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2202,6 +2309,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2402,6 +2510,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2863,10 +2972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16:M21"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2887,7 +2996,7 @@
     <col min="18" max="18" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2924,8 +3033,20 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="M1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>110</v>
       </c>
@@ -2963,13 +3084,26 @@
         <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>65</v>
+      </c>
+      <c r="O2">
+        <f>R2+5304</f>
+        <v>5304</v>
+      </c>
+      <c r="P2">
+        <v>5304</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>111</v>
       </c>
@@ -3006,14 +3140,24 @@
       <c r="L3" s="2">
         <v>57</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O15" si="0">R3+5304</f>
+        <v>5564</v>
+      </c>
+      <c r="P3" t="s">
+        <v>140</v>
+      </c>
+      <c r="R3">
         <v>260</v>
       </c>
-      <c r="N3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>111</v>
       </c>
@@ -3047,14 +3191,24 @@
       <c r="K4">
         <v>66</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>6527</v>
+      </c>
+      <c r="P4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4">
         <v>1223</v>
       </c>
-      <c r="N4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>111</v>
       </c>
@@ -3088,14 +3242,24 @@
       <c r="K5">
         <v>68</v>
       </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>6939</v>
+      </c>
+      <c r="P5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5">
         <v>1635</v>
       </c>
-      <c r="N5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>111</v>
       </c>
@@ -3123,14 +3287,24 @@
       <c r="J6">
         <v>47</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>8165</v>
+      </c>
+      <c r="P6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6">
         <v>2861</v>
       </c>
-      <c r="N6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>112</v>
       </c>
@@ -3152,14 +3326,24 @@
       <c r="G7">
         <v>53</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>8476</v>
+      </c>
+      <c r="P7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7">
         <v>3172</v>
       </c>
-      <c r="N7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>111</v>
       </c>
@@ -3178,14 +3362,24 @@
       <c r="F8">
         <v>257</v>
       </c>
-      <c r="M8">
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>8882</v>
+      </c>
+      <c r="P8" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8">
         <v>3578</v>
       </c>
-      <c r="N8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>111</v>
       </c>
@@ -3204,14 +3398,24 @@
       <c r="F9">
         <v>257</v>
       </c>
-      <c r="M9">
+      <c r="M9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>9393</v>
+      </c>
+      <c r="P9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9">
         <v>4089</v>
       </c>
-      <c r="N9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>111</v>
       </c>
@@ -3230,14 +3434,24 @@
       <c r="F10">
         <v>257</v>
       </c>
-      <c r="M10">
+      <c r="M10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>10115</v>
+      </c>
+      <c r="P10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R10">
         <v>4811</v>
       </c>
-      <c r="N10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>111</v>
       </c>
@@ -3256,14 +3470,24 @@
       <c r="F11">
         <v>257</v>
       </c>
-      <c r="M11">
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>10624</v>
+      </c>
+      <c r="P11" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11">
         <v>5320</v>
       </c>
-      <c r="N11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>111</v>
       </c>
@@ -3282,14 +3506,24 @@
       <c r="F12">
         <v>257</v>
       </c>
-      <c r="M12">
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>11030</v>
+      </c>
+      <c r="P12" t="s">
+        <v>81</v>
+      </c>
+      <c r="R12">
         <v>5726</v>
       </c>
-      <c r="N12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>111</v>
       </c>
@@ -3308,14 +3542,24 @@
       <c r="F13">
         <v>257</v>
       </c>
-      <c r="M13">
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>11344</v>
+      </c>
+      <c r="P13" t="s">
+        <v>82</v>
+      </c>
+      <c r="R13">
         <v>6040</v>
       </c>
-      <c r="N13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>111</v>
       </c>
@@ -3334,14 +3578,24 @@
       <c r="F14">
         <v>257</v>
       </c>
-      <c r="M14">
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>12667</v>
+      </c>
+      <c r="P14" t="s">
+        <v>83</v>
+      </c>
+      <c r="R14">
         <v>7363</v>
       </c>
-      <c r="N14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>111</v>
       </c>
@@ -3360,14 +3614,24 @@
       <c r="F15">
         <v>257</v>
       </c>
-      <c r="M15">
+      <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>13491</v>
+      </c>
+      <c r="P15" t="s">
+        <v>84</v>
+      </c>
+      <c r="R15">
         <v>8187</v>
       </c>
-      <c r="N15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>111</v>
       </c>
@@ -3386,8 +3650,11 @@
       <c r="F16">
         <v>257</v>
       </c>
+      <c r="M16" t="s">
+        <v>26</v>
+      </c>
       <c r="N16" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -3409,8 +3676,11 @@
       <c r="F17">
         <v>257</v>
       </c>
+      <c r="M17" t="s">
+        <v>27</v>
+      </c>
       <c r="N17" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -3432,8 +3702,11 @@
       <c r="F18">
         <v>257</v>
       </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
       <c r="N18" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -3455,8 +3728,11 @@
       <c r="F19">
         <v>257</v>
       </c>
+      <c r="M19" t="s">
+        <v>29</v>
+      </c>
       <c r="N19" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -3478,8 +3754,11 @@
       <c r="F20">
         <v>256</v>
       </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
       <c r="N20" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -3501,8 +3780,11 @@
       <c r="F21">
         <v>257</v>
       </c>
+      <c r="M21" t="s">
+        <v>31</v>
+      </c>
       <c r="N21" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -3525,10 +3807,10 @@
         <v>256</v>
       </c>
       <c r="M22" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="N22" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -3551,10 +3833,10 @@
         <v>256</v>
       </c>
       <c r="M23" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="N23" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -3577,10 +3859,10 @@
         <v>257</v>
       </c>
       <c r="M24" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="N24" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -3603,10 +3885,10 @@
         <v>257</v>
       </c>
       <c r="M25" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="N25" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -3629,10 +3911,10 @@
         <v>257</v>
       </c>
       <c r="M26" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="N26" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -3655,10 +3937,10 @@
         <v>256</v>
       </c>
       <c r="M27" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="N27" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -3681,10 +3963,10 @@
         <v>256</v>
       </c>
       <c r="M28" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="N28" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -3707,10 +3989,10 @@
         <v>256</v>
       </c>
       <c r="M29" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="N29" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -3733,10 +4015,10 @@
         <v>256</v>
       </c>
       <c r="M30" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="N30" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -3759,10 +4041,10 @@
         <v>257</v>
       </c>
       <c r="M31" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="N31" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -3785,10 +4067,10 @@
         <v>256</v>
       </c>
       <c r="M32" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="N32" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -3811,10 +4093,10 @@
         <v>256</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="N33" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -3837,10 +4119,10 @@
         <v>255</v>
       </c>
       <c r="M34" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N34" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3863,10 +4145,10 @@
         <v>256</v>
       </c>
       <c r="M35" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="N35" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -3889,10 +4171,10 @@
         <v>257</v>
       </c>
       <c r="M36" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="N36" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -3915,10 +4197,10 @@
         <v>257</v>
       </c>
       <c r="M37" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="N37" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -3941,10 +4223,10 @@
         <v>258</v>
       </c>
       <c r="M38" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="N38" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -3967,10 +4249,10 @@
         <v>258</v>
       </c>
       <c r="M39" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="N39" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -3993,10 +4275,10 @@
         <v>257</v>
       </c>
       <c r="M40" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="N40" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -4019,10 +4301,10 @@
         <v>257</v>
       </c>
       <c r="M41" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="N41" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -4045,10 +4327,10 @@
         <v>258</v>
       </c>
       <c r="M42" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="N42" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -4071,10 +4353,10 @@
         <v>260</v>
       </c>
       <c r="M43" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="N43" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -4097,10 +4379,10 @@
         <v>260</v>
       </c>
       <c r="M44" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="N44" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -4123,10 +4405,10 @@
         <v>261</v>
       </c>
       <c r="M45" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="N45" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -4149,10 +4431,10 @@
         <v>262</v>
       </c>
       <c r="M46" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="N46" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -4175,10 +4457,10 @@
         <v>261</v>
       </c>
       <c r="M47" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="N47" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -4201,10 +4483,10 @@
         <v>262</v>
       </c>
       <c r="M48" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="N48" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -4227,10 +4509,10 @@
         <v>263</v>
       </c>
       <c r="M49" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="N49" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -4253,10 +4535,10 @@
         <v>263</v>
       </c>
       <c r="M50" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="N50" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -4279,10 +4561,10 @@
         <v>263</v>
       </c>
       <c r="M51" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="N51" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -4305,10 +4587,10 @@
         <v>263</v>
       </c>
       <c r="M52" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="N52" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -4331,10 +4613,10 @@
         <v>263</v>
       </c>
       <c r="M53" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="N53" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -4357,10 +4639,10 @@
         <v>263</v>
       </c>
       <c r="M54" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -4383,7 +4665,7 @@
         <v>263</v>
       </c>
       <c r="N55" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -4406,7 +4688,7 @@
         <v>263</v>
       </c>
       <c r="N56" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -4429,7 +4711,7 @@
         <v>263</v>
       </c>
       <c r="N57" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -4452,7 +4734,7 @@
         <v>263</v>
       </c>
       <c r="N58" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -4475,7 +4757,7 @@
         <v>263</v>
       </c>
       <c r="N59" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -4498,7 +4780,7 @@
         <v>263</v>
       </c>
       <c r="N60" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -4521,67 +4803,67 @@
         <v>263</v>
       </c>
       <c r="N61" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="N62" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="N63" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:14">
       <c r="N64" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="14:14">
       <c r="N65" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="14:14">
       <c r="N66" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="14:14">
       <c r="N67" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="14:14">
       <c r="N68" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="14:14">
       <c r="N69" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="14:14">
       <c r="N70" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="14:14">
       <c r="N71" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="14:14">
       <c r="N72" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="14:14">
       <c r="N73" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>